<commit_message>
FUNCIONA EL DESCARGAR CSM
</commit_message>
<xml_diff>
--- a/home/static/xlsxs/hojaTrabajo.xlsx
+++ b/home/static/xlsxs/hojaTrabajo.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="E1" t="inlineStr">
         <is>
-          <t>MES 2</t>
+          <t>MES 4</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -502,25 +502,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>458883998.89</v>
+        <v>483148143.2</v>
       </c>
       <c r="D3" t="n">
-        <v>457007937.67</v>
+        <v>481469708.82</v>
       </c>
       <c r="E3" t="n">
-        <v>14354334.27</v>
+        <v>9909810.039999999</v>
       </c>
       <c r="F3" t="n">
-        <v>13887646.81</v>
+        <v>10574124.34</v>
       </c>
       <c r="G3" t="n">
-        <v>473238333.16</v>
+        <v>493057953.24</v>
       </c>
       <c r="H3" t="n">
-        <v>470895584.48</v>
+        <v>492043833.16</v>
       </c>
       <c r="I3" t="n">
-        <v>2342748.68</v>
+        <v>1014120.08</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -538,25 +538,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>182844487.91</v>
+        <v>190634942.43</v>
       </c>
       <c r="D4" t="n">
-        <v>178115283.78</v>
+        <v>187382795.66</v>
       </c>
       <c r="E4" t="n">
-        <v>4288949.7</v>
+        <v>3501504.82</v>
       </c>
       <c r="F4" t="n">
-        <v>6000085.75</v>
+        <v>3267426.13</v>
       </c>
       <c r="G4" t="n">
-        <v>187133437.61</v>
+        <v>194136447.25</v>
       </c>
       <c r="H4" t="n">
-        <v>184115369.53</v>
+        <v>190650221.79</v>
       </c>
       <c r="I4" t="n">
-        <v>3018068.08</v>
+        <v>3486225.46</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -574,25 +574,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3388150.52</v>
+        <v>3522959.97</v>
       </c>
       <c r="D5" t="n">
-        <v>3108324.57</v>
+        <v>3233940.31</v>
       </c>
       <c r="E5" t="n">
-        <v>66212.32000000001</v>
+        <v>68597.13</v>
       </c>
       <c r="F5" t="n">
-        <v>64024.96</v>
+        <v>61590.78</v>
       </c>
       <c r="G5" t="n">
-        <v>3454362.84</v>
+        <v>3591557.1</v>
       </c>
       <c r="H5" t="n">
-        <v>3172349.53</v>
+        <v>3295531.09</v>
       </c>
       <c r="I5" t="n">
-        <v>282013.31</v>
+        <v>296026.01</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>5207361.52</v>
       </c>
       <c r="D6" t="n">
-        <v>3392526.6</v>
+        <v>3401113.67</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>7894.67</v>
+        <v>692.4</v>
       </c>
       <c r="G6" t="n">
         <v>5207361.52</v>
       </c>
       <c r="H6" t="n">
-        <v>3400421.27</v>
+        <v>3401806.07</v>
       </c>
       <c r="I6" t="n">
-        <v>1806940.25</v>
+        <v>1805555.45</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -646,28 +646,28 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8990266.93</v>
+        <v>9534611.4</v>
       </c>
       <c r="D7" t="n">
-        <v>9976259.5</v>
+        <v>10463223.64</v>
       </c>
       <c r="E7" t="n">
-        <v>284371.73</v>
+        <v>259972.74</v>
       </c>
       <c r="F7" t="n">
-        <v>243566.64</v>
+        <v>243397.5</v>
       </c>
       <c r="G7" t="n">
-        <v>9274638.66</v>
+        <v>9794584.140000001</v>
       </c>
       <c r="H7" t="n">
-        <v>10219826.14</v>
+        <v>10706621.14</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>945187.48</v>
+        <v>912037</v>
       </c>
     </row>
     <row r="8">
@@ -682,25 +682,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>39056795.32</v>
+        <v>39106870.99</v>
       </c>
       <c r="D8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="E8" t="n">
-        <v>1725.99</v>
+        <v>48349.68</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>39058521.31</v>
+        <v>39155220.67</v>
       </c>
       <c r="H8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="I8" t="n">
-        <v>27930785.9</v>
+        <v>28027485.26</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -718,25 +718,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>44797256.3</v>
+        <v>45811120.84</v>
       </c>
       <c r="D9" t="n">
-        <v>40222506.1</v>
+        <v>41331171.15</v>
       </c>
       <c r="E9" t="n">
-        <v>485946.63</v>
+        <v>527917.91</v>
       </c>
       <c r="F9" t="n">
-        <v>507327.02</v>
+        <v>601338.03</v>
       </c>
       <c r="G9" t="n">
-        <v>45283202.93</v>
+        <v>46339038.75</v>
       </c>
       <c r="H9" t="n">
-        <v>40729833.12</v>
+        <v>41932509.18</v>
       </c>
       <c r="I9" t="n">
-        <v>4553369.81</v>
+        <v>4406529.57</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -757,25 +757,25 @@
         <v>10298822.64</v>
       </c>
       <c r="D10" t="n">
-        <v>33884520.99</v>
+        <v>35185144.84</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>665975.51</v>
+        <v>634648.34</v>
       </c>
       <c r="G10" t="n">
         <v>10298822.64</v>
       </c>
       <c r="H10" t="n">
-        <v>34550496.5</v>
+        <v>35819793.18</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>24251673.86</v>
+        <v>25520970.54</v>
       </c>
     </row>
     <row r="11">
@@ -790,28 +790,28 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>27834003.26</v>
+        <v>29489652.82</v>
       </c>
       <c r="D11" t="n">
-        <v>29222947.21</v>
+        <v>30779593.07</v>
       </c>
       <c r="E11" t="n">
-        <v>751813.51</v>
+        <v>903836.05</v>
       </c>
       <c r="F11" t="n">
-        <v>840303.54</v>
+        <v>716342.3199999999</v>
       </c>
       <c r="G11" t="n">
-        <v>28585816.77</v>
+        <v>30393488.87</v>
       </c>
       <c r="H11" t="n">
-        <v>30063250.75</v>
+        <v>31495935.39</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1477433.98</v>
+        <v>1102446.52</v>
       </c>
     </row>
     <row r="12">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21695338.93</v>
+        <v>22416323.67</v>
       </c>
       <c r="D12" t="n">
-        <v>20780250.7</v>
+        <v>21604592.34</v>
       </c>
       <c r="E12" t="n">
-        <v>411219.28</v>
+        <v>309765.46</v>
       </c>
       <c r="F12" t="n">
-        <v>460280.22</v>
+        <v>364061.42</v>
       </c>
       <c r="G12" t="n">
-        <v>22106558.21</v>
+        <v>22726089.13</v>
       </c>
       <c r="H12" t="n">
-        <v>21240530.92</v>
+        <v>21968653.76</v>
       </c>
       <c r="I12" t="n">
-        <v>866027.29</v>
+        <v>757435.37</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -862,28 +862,28 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>104911482.26</v>
+        <v>109071433.52</v>
       </c>
       <c r="D13" t="n">
-        <v>105859930.59</v>
+        <v>110129871.63</v>
       </c>
       <c r="E13" t="n">
-        <v>1766013.15</v>
+        <v>2393938.11</v>
       </c>
       <c r="F13" t="n">
-        <v>2029150.24</v>
+        <v>2240790.8</v>
       </c>
       <c r="G13" t="n">
-        <v>106677495.41</v>
+        <v>111465371.63</v>
       </c>
       <c r="H13" t="n">
-        <v>107889080.83</v>
+        <v>112370662.43</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1211585.42</v>
+        <v>905290.8</v>
       </c>
     </row>
     <row r="14">
@@ -898,28 +898,28 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>41178536.92</v>
+        <v>44805507.88</v>
       </c>
       <c r="D14" t="n">
-        <v>58092326.73</v>
+        <v>58226524.29</v>
       </c>
       <c r="E14" t="n">
-        <v>2926130.83</v>
+        <v>700840.13</v>
       </c>
       <c r="F14" t="n">
-        <v>73599.17999999999</v>
+        <v>60598.38</v>
       </c>
       <c r="G14" t="n">
-        <v>44104667.75</v>
+        <v>45506348.01</v>
       </c>
       <c r="H14" t="n">
-        <v>58165925.91</v>
+        <v>58287122.67</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>14061258.16</v>
+        <v>12780774.66</v>
       </c>
     </row>
     <row r="15">
@@ -934,25 +934,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1858427.9</v>
+        <v>1925148.37</v>
       </c>
       <c r="D15" t="n">
-        <v>1833941.95</v>
+        <v>1901416.88</v>
       </c>
       <c r="E15" t="n">
-        <v>35176.91</v>
+        <v>31543.56</v>
       </c>
       <c r="F15" t="n">
-        <v>35449.63</v>
+        <v>32025.3</v>
       </c>
       <c r="G15" t="n">
-        <v>1893604.81</v>
+        <v>1956691.93</v>
       </c>
       <c r="H15" t="n">
-        <v>1869391.58</v>
+        <v>1933442.18</v>
       </c>
       <c r="I15" t="n">
-        <v>24213.23</v>
+        <v>23249.75</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -970,25 +970,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1020741.64</v>
+        <v>3032007.04</v>
       </c>
       <c r="D16" t="n">
-        <v>20269.33</v>
+        <v>77017.57000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>927152.8100000001</v>
+        <v>1084112.59</v>
       </c>
       <c r="F16" t="n">
-        <v>24700.51</v>
+        <v>32047.73</v>
       </c>
       <c r="G16" t="n">
-        <v>1947894.45</v>
+        <v>4116119.63</v>
       </c>
       <c r="H16" t="n">
-        <v>44969.84</v>
+        <v>109065.3</v>
       </c>
       <c r="I16" t="n">
-        <v>1902924.61</v>
+        <v>4007054.33</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1006,28 +1006,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>166828.64</v>
+        <v>654362.75</v>
       </c>
       <c r="D17" t="n">
-        <v>124426.08</v>
+        <v>668770.55</v>
       </c>
       <c r="E17" t="n">
-        <v>243566.64</v>
+        <v>243967.47</v>
       </c>
       <c r="F17" t="n">
-        <v>284371.73</v>
+        <v>259972.74</v>
       </c>
       <c r="G17" t="n">
-        <v>410395.28</v>
+        <v>898330.22</v>
       </c>
       <c r="H17" t="n">
-        <v>408797.81</v>
+        <v>928743.29</v>
       </c>
       <c r="I17" t="n">
-        <v>1597.47</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>30413.07</v>
       </c>
     </row>
     <row r="18">
@@ -1042,25 +1042,25 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>676294.02</v>
+        <v>1661343.48</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>538887.27</v>
+        <v>446162.19</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>1215181.29</v>
+        <v>2107505.67</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>1215181.29</v>
+        <v>2107505.67</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1078,25 +1078,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>702241.87</v>
+        <v>2027135.58</v>
       </c>
       <c r="D19" t="n">
         <v>133163.83</v>
       </c>
       <c r="E19" t="n">
-        <v>720597.5</v>
+        <v>604296.21</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>1422839.37</v>
+        <v>2631431.79</v>
       </c>
       <c r="H19" t="n">
         <v>133163.83</v>
       </c>
       <c r="I19" t="n">
-        <v>1289675.54</v>
+        <v>2498267.96</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1114,25 +1114,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9386.190000000001</v>
+        <v>79157.74000000001</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>10867.81</v>
+        <v>58903.74</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>20254</v>
+        <v>138061.48</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>20254</v>
+        <v>138061.48</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1150,25 +1150,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>96761.45</v>
+        <v>337641.88</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>121737.77</v>
+        <v>119142.66</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>218499.22</v>
+        <v>456784.54</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>218499.22</v>
+        <v>456784.54</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1186,25 +1186,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>321748.82</v>
+        <v>628545.14</v>
       </c>
       <c r="D22" t="n">
         <v>10561</v>
       </c>
       <c r="E22" t="n">
-        <v>166275.63</v>
+        <v>140520.69</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>488024.45</v>
+        <v>769065.83</v>
       </c>
       <c r="H22" t="n">
         <v>10561</v>
       </c>
       <c r="I22" t="n">
-        <v>477463.45</v>
+        <v>758504.83</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1222,25 +1222,25 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>783437.09</v>
+        <v>2286579.96</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>771950.41</v>
+        <v>731192.46</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1555387.5</v>
+        <v>3017772.42</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>1555387.5</v>
+        <v>3017772.42</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1261,25 +1261,25 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>3303231.16</v>
+        <v>8155756.43</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>2048860.39</v>
+        <v>2803664.88</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>5352091.55</v>
+        <v>10959421.31</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>5352091.55</v>
+        <v>10959421.31</v>
       </c>
     </row>
     <row r="25">
@@ -1297,25 +1297,25 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>14414.08</v>
+        <v>52353.38</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>16192.93</v>
+        <v>21746.37</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>30607.01</v>
+        <v>74099.75</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>30607.01</v>
+        <v>74099.75</v>
       </c>
     </row>
     <row r="26">
@@ -1333,25 +1333,25 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1650795.62</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1529205.62</v>
+        <v>121590</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1529205.62</v>
+        <v>1772385.62</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>1529205.62</v>
+        <v>1772385.62</v>
       </c>
     </row>
     <row r="27">
@@ -1369,25 +1369,25 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>2607.94</v>
+        <v>205218.93</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>154294.81</v>
+        <v>48316.18</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>156902.75</v>
+        <v>253535.11</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>156902.75</v>
+        <v>253535.11</v>
       </c>
     </row>
     <row r="28">
@@ -1405,25 +1405,25 @@
         <v>143724.83</v>
       </c>
       <c r="D28" t="n">
-        <v>3632744.31</v>
+        <v>9960985.439999999</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>3191963.6</v>
+        <v>3136277.53</v>
       </c>
       <c r="G28" t="n">
         <v>143724.83</v>
       </c>
       <c r="H28" t="n">
-        <v>6824707.91</v>
+        <v>13097262.97</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>6680983.08</v>
+        <v>12953538.14</v>
       </c>
     </row>
     <row r="29">
@@ -1438,25 +1438,25 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3010648.52</v>
+        <v>8382729.65</v>
       </c>
       <c r="D29" t="n">
         <v>133163.83</v>
       </c>
       <c r="E29" t="n">
-        <v>2710126.79</v>
+        <v>2661954.34</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>5720775.31</v>
+        <v>11044683.99</v>
       </c>
       <c r="H29" t="n">
         <v>133163.83</v>
       </c>
       <c r="I29" t="n">
-        <v>5587611.48</v>
+        <v>10911520.16</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1474,25 +1474,25 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>142006.19</v>
+        <v>482619.93</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>153027.81</v>
+        <v>187585.93</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>295034</v>
+        <v>670205.86</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>295034</v>
+        <v>670205.86</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1510,25 +1510,25 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>158340.78</v>
+        <v>467090.73</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>162533.37</v>
+        <v>146216.58</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>320874.15</v>
+        <v>613307.3100000001</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>320874.15</v>
+        <v>613307.3100000001</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -1546,25 +1546,25 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>321748.82</v>
+        <v>628545.13</v>
       </c>
       <c r="D32" t="n">
         <v>10561</v>
       </c>
       <c r="E32" t="n">
-        <v>166275.63</v>
+        <v>140520.68</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>488024.45</v>
+        <v>769065.8100000001</v>
       </c>
       <c r="H32" t="n">
         <v>10561</v>
       </c>
       <c r="I32" t="n">
-        <v>477463.45</v>
+        <v>758504.8100000001</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1594,16 +1594,16 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>990563731.92</v>
+        <v>1041005034.26</v>
       </c>
       <c r="H33" t="n">
-        <v>992074528.12</v>
+        <v>1042515830.46</v>
       </c>
       <c r="I33" t="n">
-        <v>54186132.71</v>
+        <v>65754116.32</v>
       </c>
       <c r="J33" t="n">
-        <v>55696928.91</v>
+        <v>67264912.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se soluciono un bug y ademas se manda ya los datos
</commit_message>
<xml_diff>
--- a/home/static/xlsxs/hojaTrabajo.xlsx
+++ b/home/static/xlsxs/hojaTrabajo.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="E1" t="inlineStr">
         <is>
-          <t>MES 4</t>
+          <t>MES 1</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -502,25 +502,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>483148143.2</v>
+        <v>446858039.41</v>
       </c>
       <c r="D3" t="n">
-        <v>481469708.82</v>
+        <v>444564133.25</v>
       </c>
       <c r="E3" t="n">
-        <v>9909810.039999999</v>
+        <v>12025959.48</v>
       </c>
       <c r="F3" t="n">
-        <v>10574124.34</v>
+        <v>12443804.42</v>
       </c>
       <c r="G3" t="n">
-        <v>493057953.24</v>
+        <v>458883998.89</v>
       </c>
       <c r="H3" t="n">
-        <v>492043833.16</v>
+        <v>457007937.67</v>
       </c>
       <c r="I3" t="n">
-        <v>1014120.08</v>
+        <v>1876061.22</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -538,25 +538,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>190634942.43</v>
+        <v>178898149.91</v>
       </c>
       <c r="D4" t="n">
-        <v>187382795.66</v>
+        <v>174836588.82</v>
       </c>
       <c r="E4" t="n">
-        <v>3501504.82</v>
+        <v>3946338</v>
       </c>
       <c r="F4" t="n">
-        <v>3267426.13</v>
+        <v>3278694.96</v>
       </c>
       <c r="G4" t="n">
-        <v>194136447.25</v>
+        <v>182844487.91</v>
       </c>
       <c r="H4" t="n">
-        <v>190650221.79</v>
+        <v>178115283.78</v>
       </c>
       <c r="I4" t="n">
-        <v>3486225.46</v>
+        <v>4729204.13</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -574,25 +574,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3522959.97</v>
+        <v>3315868.6</v>
       </c>
       <c r="D5" t="n">
-        <v>3233940.31</v>
+        <v>3030695.5</v>
       </c>
       <c r="E5" t="n">
-        <v>68597.13</v>
+        <v>72281.92</v>
       </c>
       <c r="F5" t="n">
-        <v>61590.78</v>
+        <v>77629.07000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>3591557.1</v>
+        <v>3388150.52</v>
       </c>
       <c r="H5" t="n">
-        <v>3295531.09</v>
+        <v>3108324.57</v>
       </c>
       <c r="I5" t="n">
-        <v>296026.01</v>
+        <v>279825.95</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>5207361.52</v>
       </c>
       <c r="D6" t="n">
-        <v>3401113.67</v>
+        <v>3392032.96</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>692.4</v>
+        <v>493.64</v>
       </c>
       <c r="G6" t="n">
         <v>5207361.52</v>
       </c>
       <c r="H6" t="n">
-        <v>3401806.07</v>
+        <v>3392526.6</v>
       </c>
       <c r="I6" t="n">
-        <v>1805555.45</v>
+        <v>1814834.92</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -646,28 +646,28 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9534611.4</v>
+        <v>8865840.85</v>
       </c>
       <c r="D7" t="n">
-        <v>10463223.64</v>
+        <v>9809430.859999999</v>
       </c>
       <c r="E7" t="n">
-        <v>259972.74</v>
+        <v>124426.08</v>
       </c>
       <c r="F7" t="n">
-        <v>243397.5</v>
+        <v>166828.64</v>
       </c>
       <c r="G7" t="n">
-        <v>9794584.140000001</v>
+        <v>8990266.93</v>
       </c>
       <c r="H7" t="n">
-        <v>10706621.14</v>
+        <v>9976259.5</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>912037</v>
+        <v>985992.5699999999</v>
       </c>
     </row>
     <row r="8">
@@ -682,25 +682,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>39106870.99</v>
+        <v>38965131.09</v>
       </c>
       <c r="D8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="E8" t="n">
-        <v>48349.68</v>
+        <v>91664.23</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>39155220.67</v>
+        <v>39056795.32</v>
       </c>
       <c r="H8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="I8" t="n">
-        <v>28027485.26</v>
+        <v>27929059.91</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -718,25 +718,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>45811120.84</v>
+        <v>44084628.02</v>
       </c>
       <c r="D9" t="n">
-        <v>41331171.15</v>
+        <v>39554245.57</v>
       </c>
       <c r="E9" t="n">
-        <v>527917.91</v>
+        <v>712628.28</v>
       </c>
       <c r="F9" t="n">
-        <v>601338.03</v>
+        <v>668260.53</v>
       </c>
       <c r="G9" t="n">
-        <v>46339038.75</v>
+        <v>44797256.3</v>
       </c>
       <c r="H9" t="n">
-        <v>41932509.18</v>
+        <v>40222506.1</v>
       </c>
       <c r="I9" t="n">
-        <v>4406529.57</v>
+        <v>4574750.2</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -757,25 +757,25 @@
         <v>10298822.64</v>
       </c>
       <c r="D10" t="n">
-        <v>35185144.84</v>
+        <v>33218458.2</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>634648.34</v>
+        <v>666062.79</v>
       </c>
       <c r="G10" t="n">
         <v>10298822.64</v>
       </c>
       <c r="H10" t="n">
-        <v>35819793.18</v>
+        <v>33884520.99</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>25520970.54</v>
+        <v>23585698.35</v>
       </c>
     </row>
     <row r="11">
@@ -790,28 +790,28 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>29489652.82</v>
+        <v>26927488.81</v>
       </c>
       <c r="D11" t="n">
-        <v>30779593.07</v>
+        <v>28418236.51</v>
       </c>
       <c r="E11" t="n">
-        <v>903836.05</v>
+        <v>906514.45</v>
       </c>
       <c r="F11" t="n">
-        <v>716342.3199999999</v>
+        <v>804710.7</v>
       </c>
       <c r="G11" t="n">
-        <v>30393488.87</v>
+        <v>27834003.26</v>
       </c>
       <c r="H11" t="n">
-        <v>31495935.39</v>
+        <v>29222947.21</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1102446.52</v>
+        <v>1388943.95</v>
       </c>
     </row>
     <row r="12">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22416323.67</v>
+        <v>21194001.89</v>
       </c>
       <c r="D12" t="n">
-        <v>21604592.34</v>
+        <v>20218012.67</v>
       </c>
       <c r="E12" t="n">
-        <v>309765.46</v>
+        <v>501337.04</v>
       </c>
       <c r="F12" t="n">
-        <v>364061.42</v>
+        <v>562238.03</v>
       </c>
       <c r="G12" t="n">
-        <v>22726089.13</v>
+        <v>21695338.93</v>
       </c>
       <c r="H12" t="n">
-        <v>21968653.76</v>
+        <v>20780250.7</v>
       </c>
       <c r="I12" t="n">
-        <v>757435.37</v>
+        <v>915088.23</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -862,28 +862,28 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>109071433.52</v>
+        <v>102812310.62</v>
       </c>
       <c r="D13" t="n">
-        <v>110129871.63</v>
+        <v>103576692.79</v>
       </c>
       <c r="E13" t="n">
-        <v>2393938.11</v>
+        <v>2099171.64</v>
       </c>
       <c r="F13" t="n">
-        <v>2240790.8</v>
+        <v>2283237.8</v>
       </c>
       <c r="G13" t="n">
-        <v>111465371.63</v>
+        <v>104911482.26</v>
       </c>
       <c r="H13" t="n">
-        <v>112370662.43</v>
+        <v>105859930.59</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>905290.8</v>
+        <v>948448.33</v>
       </c>
     </row>
     <row r="14">
@@ -898,28 +898,28 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>44805507.88</v>
+        <v>40628716.89</v>
       </c>
       <c r="D14" t="n">
-        <v>58226524.29</v>
+        <v>57808813.4</v>
       </c>
       <c r="E14" t="n">
-        <v>700840.13</v>
+        <v>549820.03</v>
       </c>
       <c r="F14" t="n">
-        <v>60598.38</v>
+        <v>283513.33</v>
       </c>
       <c r="G14" t="n">
-        <v>45506348.01</v>
+        <v>41178536.92</v>
       </c>
       <c r="H14" t="n">
-        <v>58287122.67</v>
+        <v>58092326.73</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>12780774.66</v>
+        <v>16913789.81</v>
       </c>
     </row>
     <row r="15">
@@ -934,25 +934,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1925148.37</v>
+        <v>1782949.13</v>
       </c>
       <c r="D15" t="n">
-        <v>1901416.88</v>
+        <v>1795029.64</v>
       </c>
       <c r="E15" t="n">
-        <v>31543.56</v>
+        <v>75478.77</v>
       </c>
       <c r="F15" t="n">
-        <v>32025.3</v>
+        <v>38912.31</v>
       </c>
       <c r="G15" t="n">
-        <v>1956691.93</v>
+        <v>1858427.9</v>
       </c>
       <c r="H15" t="n">
-        <v>1933442.18</v>
+        <v>1833941.95</v>
       </c>
       <c r="I15" t="n">
-        <v>23249.75</v>
+        <v>24485.95</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -970,25 +970,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3032007.04</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>77017.57000000001</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1084112.59</v>
+        <v>1020741.64</v>
       </c>
       <c r="F16" t="n">
-        <v>32047.73</v>
+        <v>20269.33</v>
       </c>
       <c r="G16" t="n">
-        <v>4116119.63</v>
+        <v>1020741.64</v>
       </c>
       <c r="H16" t="n">
-        <v>109065.3</v>
+        <v>20269.33</v>
       </c>
       <c r="I16" t="n">
-        <v>4007054.33</v>
+        <v>1000472.31</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1006,28 +1006,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>654362.75</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>668770.55</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>243967.47</v>
+        <v>166828.64</v>
       </c>
       <c r="F17" t="n">
-        <v>259972.74</v>
+        <v>124426.08</v>
       </c>
       <c r="G17" t="n">
-        <v>898330.22</v>
+        <v>166828.64</v>
       </c>
       <c r="H17" t="n">
-        <v>928743.29</v>
+        <v>124426.08</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>42402.56</v>
       </c>
       <c r="J17" t="n">
-        <v>30413.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1042,25 +1042,25 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1661343.48</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>446162.19</v>
+        <v>676294.02</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>2107505.67</v>
+        <v>676294.02</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>2107505.67</v>
+        <v>676294.02</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1078,25 +1078,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2027135.58</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>702241.87</v>
+      </c>
+      <c r="F19" t="n">
         <v>133163.83</v>
       </c>
-      <c r="E19" t="n">
-        <v>604296.21</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
       <c r="G19" t="n">
-        <v>2631431.79</v>
+        <v>702241.87</v>
       </c>
       <c r="H19" t="n">
         <v>133163.83</v>
       </c>
       <c r="I19" t="n">
-        <v>2498267.96</v>
+        <v>569078.04</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1114,25 +1114,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>79157.74000000001</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>58903.74</v>
+        <v>9386.190000000001</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>138061.48</v>
+        <v>9386.190000000001</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>138061.48</v>
+        <v>9386.190000000001</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1150,25 +1150,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>337641.88</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>119142.66</v>
+        <v>96761.45</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>456784.54</v>
+        <v>96761.45</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>456784.54</v>
+        <v>96761.45</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1186,25 +1186,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>628545.14</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>321748.82</v>
+      </c>
+      <c r="F22" t="n">
         <v>10561</v>
       </c>
-      <c r="E22" t="n">
-        <v>140520.69</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
       <c r="G22" t="n">
-        <v>769065.83</v>
+        <v>321748.82</v>
       </c>
       <c r="H22" t="n">
         <v>10561</v>
       </c>
       <c r="I22" t="n">
-        <v>758504.83</v>
+        <v>311187.82</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1222,25 +1222,25 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2286579.96</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>731192.46</v>
+        <v>783437.09</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>3017772.42</v>
+        <v>783437.09</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>3017772.42</v>
+        <v>783437.09</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1261,25 +1261,25 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>8155756.43</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>2803664.88</v>
+        <v>3303231.16</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>10959421.31</v>
+        <v>3303231.16</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>10959421.31</v>
+        <v>3303231.16</v>
       </c>
     </row>
     <row r="25">
@@ -1297,25 +1297,25 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>52353.38</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>21746.37</v>
+        <v>14414.08</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>74099.75</v>
+        <v>14414.08</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>74099.75</v>
+        <v>14414.08</v>
       </c>
     </row>
     <row r="26">
@@ -1333,25 +1333,25 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>1650795.62</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>121590</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1772385.62</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>1772385.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1369,25 +1369,25 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>205218.93</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>48316.18</v>
+        <v>2607.94</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>253535.11</v>
+        <v>2607.94</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>253535.11</v>
+        <v>2607.94</v>
       </c>
     </row>
     <row r="28">
@@ -1402,28 +1402,28 @@
         </is>
       </c>
       <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
         <v>143724.83</v>
       </c>
-      <c r="D28" t="n">
-        <v>9960985.439999999</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
       <c r="F28" t="n">
-        <v>3136277.53</v>
+        <v>3632744.31</v>
       </c>
       <c r="G28" t="n">
         <v>143724.83</v>
       </c>
       <c r="H28" t="n">
-        <v>13097262.97</v>
+        <v>3632744.31</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>12953538.14</v>
+        <v>3489019.48</v>
       </c>
     </row>
     <row r="29">
@@ -1438,25 +1438,25 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>8382729.65</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3010648.52</v>
+      </c>
+      <c r="F29" t="n">
         <v>133163.83</v>
       </c>
-      <c r="E29" t="n">
-        <v>2661954.34</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
       <c r="G29" t="n">
-        <v>11044683.99</v>
+        <v>3010648.52</v>
       </c>
       <c r="H29" t="n">
         <v>133163.83</v>
       </c>
       <c r="I29" t="n">
-        <v>10911520.16</v>
+        <v>2877484.69</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1474,25 +1474,25 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>482619.93</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>187585.93</v>
+        <v>142006.19</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>670205.86</v>
+        <v>142006.19</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>670205.86</v>
+        <v>142006.19</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1510,25 +1510,25 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>467090.73</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>146216.58</v>
+        <v>158340.78</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>613307.3100000001</v>
+        <v>158340.78</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>613307.3100000001</v>
+        <v>158340.78</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -1546,25 +1546,25 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>628545.13</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>321748.82</v>
+      </c>
+      <c r="F32" t="n">
         <v>10561</v>
       </c>
-      <c r="E32" t="n">
-        <v>140520.68</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
       <c r="G32" t="n">
-        <v>769065.8100000001</v>
+        <v>321748.82</v>
       </c>
       <c r="H32" t="n">
         <v>10561</v>
       </c>
       <c r="I32" t="n">
-        <v>758504.8100000001</v>
+        <v>311187.82</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1594,16 +1594,16 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>1041005034.26</v>
+        <v>958498838.16</v>
       </c>
       <c r="H33" t="n">
-        <v>1042515830.46</v>
+        <v>960009634.36</v>
       </c>
       <c r="I33" t="n">
-        <v>65754116.32</v>
+        <v>49121349.47</v>
       </c>
       <c r="J33" t="n">
-        <v>67264912.52</v>
+        <v>50632145.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregue disenio culebro al trabajo
</commit_message>
<xml_diff>
--- a/home/static/xlsxs/hojaTrabajo.xlsx
+++ b/home/static/xlsxs/hojaTrabajo.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="E1" t="inlineStr">
         <is>
-          <t>MES 1</t>
+          <t>MES 3</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -502,25 +502,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>446858039.41</v>
+        <v>473238333.16</v>
       </c>
       <c r="D3" t="n">
-        <v>444564133.25</v>
+        <v>470895584.48</v>
       </c>
       <c r="E3" t="n">
-        <v>12025959.48</v>
+        <v>9909810.039999999</v>
       </c>
       <c r="F3" t="n">
-        <v>12443804.42</v>
+        <v>10574124.34</v>
       </c>
       <c r="G3" t="n">
-        <v>458883998.89</v>
+        <v>483148143.2</v>
       </c>
       <c r="H3" t="n">
-        <v>457007937.67</v>
+        <v>481469708.82</v>
       </c>
       <c r="I3" t="n">
-        <v>1876061.22</v>
+        <v>1678434.38</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -538,25 +538,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>178898149.91</v>
+        <v>187133437.61</v>
       </c>
       <c r="D4" t="n">
-        <v>174836588.82</v>
+        <v>184115369.53</v>
       </c>
       <c r="E4" t="n">
-        <v>3946338</v>
+        <v>3501504.82</v>
       </c>
       <c r="F4" t="n">
-        <v>3278694.96</v>
+        <v>3267426.13</v>
       </c>
       <c r="G4" t="n">
-        <v>182844487.91</v>
+        <v>190634942.43</v>
       </c>
       <c r="H4" t="n">
-        <v>178115283.78</v>
+        <v>187382795.66</v>
       </c>
       <c r="I4" t="n">
-        <v>4729204.13</v>
+        <v>3252146.77</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -574,25 +574,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3315868.6</v>
+        <v>3454362.84</v>
       </c>
       <c r="D5" t="n">
-        <v>3030695.5</v>
+        <v>3172349.53</v>
       </c>
       <c r="E5" t="n">
-        <v>72281.92</v>
+        <v>68597.13</v>
       </c>
       <c r="F5" t="n">
-        <v>77629.07000000001</v>
+        <v>61590.78</v>
       </c>
       <c r="G5" t="n">
-        <v>3388150.52</v>
+        <v>3522959.97</v>
       </c>
       <c r="H5" t="n">
-        <v>3108324.57</v>
+        <v>3233940.31</v>
       </c>
       <c r="I5" t="n">
-        <v>279825.95</v>
+        <v>289019.66</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>5207361.52</v>
       </c>
       <c r="D6" t="n">
-        <v>3392032.96</v>
+        <v>3400421.27</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>493.64</v>
+        <v>692.4</v>
       </c>
       <c r="G6" t="n">
         <v>5207361.52</v>
       </c>
       <c r="H6" t="n">
-        <v>3392526.6</v>
+        <v>3401113.67</v>
       </c>
       <c r="I6" t="n">
-        <v>1814834.92</v>
+        <v>1806247.85</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -646,28 +646,28 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8865840.85</v>
+        <v>9274638.66</v>
       </c>
       <c r="D7" t="n">
-        <v>9809430.859999999</v>
+        <v>10219826.14</v>
       </c>
       <c r="E7" t="n">
-        <v>124426.08</v>
+        <v>259972.74</v>
       </c>
       <c r="F7" t="n">
-        <v>166828.64</v>
+        <v>243397.5</v>
       </c>
       <c r="G7" t="n">
-        <v>8990266.93</v>
+        <v>9534611.4</v>
       </c>
       <c r="H7" t="n">
-        <v>9976259.5</v>
+        <v>10463223.64</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>985992.5699999999</v>
+        <v>928612.24</v>
       </c>
     </row>
     <row r="8">
@@ -682,25 +682,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>38965131.09</v>
+        <v>39058521.31</v>
       </c>
       <c r="D8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="E8" t="n">
-        <v>91664.23</v>
+        <v>48349.68</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>39056795.32</v>
+        <v>39106870.99</v>
       </c>
       <c r="H8" t="n">
         <v>11127735.41</v>
       </c>
       <c r="I8" t="n">
-        <v>27929059.91</v>
+        <v>27979135.58</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -718,25 +718,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>44084628.02</v>
+        <v>45283202.93</v>
       </c>
       <c r="D9" t="n">
-        <v>39554245.57</v>
+        <v>40729833.12</v>
       </c>
       <c r="E9" t="n">
-        <v>712628.28</v>
+        <v>527917.91</v>
       </c>
       <c r="F9" t="n">
-        <v>668260.53</v>
+        <v>601338.03</v>
       </c>
       <c r="G9" t="n">
-        <v>44797256.3</v>
+        <v>45811120.84</v>
       </c>
       <c r="H9" t="n">
-        <v>40222506.1</v>
+        <v>41331171.15</v>
       </c>
       <c r="I9" t="n">
-        <v>4574750.2</v>
+        <v>4479949.69</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -757,25 +757,25 @@
         <v>10298822.64</v>
       </c>
       <c r="D10" t="n">
-        <v>33218458.2</v>
+        <v>34550496.5</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>666062.79</v>
+        <v>634648.34</v>
       </c>
       <c r="G10" t="n">
         <v>10298822.64</v>
       </c>
       <c r="H10" t="n">
-        <v>33884520.99</v>
+        <v>35185144.84</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>23585698.35</v>
+        <v>24886322.2</v>
       </c>
     </row>
     <row r="11">
@@ -790,28 +790,28 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26927488.81</v>
+        <v>28585816.77</v>
       </c>
       <c r="D11" t="n">
-        <v>28418236.51</v>
+        <v>30063250.75</v>
       </c>
       <c r="E11" t="n">
-        <v>906514.45</v>
+        <v>903836.05</v>
       </c>
       <c r="F11" t="n">
-        <v>804710.7</v>
+        <v>716342.3199999999</v>
       </c>
       <c r="G11" t="n">
-        <v>27834003.26</v>
+        <v>29489652.82</v>
       </c>
       <c r="H11" t="n">
-        <v>29222947.21</v>
+        <v>30779593.07</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1388943.95</v>
+        <v>1289940.25</v>
       </c>
     </row>
     <row r="12">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21194001.89</v>
+        <v>22106558.21</v>
       </c>
       <c r="D12" t="n">
-        <v>20218012.67</v>
+        <v>21240530.92</v>
       </c>
       <c r="E12" t="n">
-        <v>501337.04</v>
+        <v>309765.46</v>
       </c>
       <c r="F12" t="n">
-        <v>562238.03</v>
+        <v>364061.42</v>
       </c>
       <c r="G12" t="n">
-        <v>21695338.93</v>
+        <v>22416323.67</v>
       </c>
       <c r="H12" t="n">
-        <v>20780250.7</v>
+        <v>21604592.34</v>
       </c>
       <c r="I12" t="n">
-        <v>915088.23</v>
+        <v>811731.33</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -862,28 +862,28 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>102812310.62</v>
+        <v>106677495.41</v>
       </c>
       <c r="D13" t="n">
-        <v>103576692.79</v>
+        <v>107889080.83</v>
       </c>
       <c r="E13" t="n">
-        <v>2099171.64</v>
+        <v>2393938.11</v>
       </c>
       <c r="F13" t="n">
-        <v>2283237.8</v>
+        <v>2240790.8</v>
       </c>
       <c r="G13" t="n">
-        <v>104911482.26</v>
+        <v>109071433.52</v>
       </c>
       <c r="H13" t="n">
-        <v>105859930.59</v>
+        <v>110129871.63</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>948448.33</v>
+        <v>1058438.11</v>
       </c>
     </row>
     <row r="14">
@@ -898,28 +898,28 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40628716.89</v>
+        <v>44104667.75</v>
       </c>
       <c r="D14" t="n">
-        <v>57808813.4</v>
+        <v>58165925.91</v>
       </c>
       <c r="E14" t="n">
-        <v>549820.03</v>
+        <v>700840.13</v>
       </c>
       <c r="F14" t="n">
-        <v>283513.33</v>
+        <v>60598.38</v>
       </c>
       <c r="G14" t="n">
-        <v>41178536.92</v>
+        <v>44805507.88</v>
       </c>
       <c r="H14" t="n">
-        <v>58092326.73</v>
+        <v>58226524.29</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>16913789.81</v>
+        <v>13421016.41</v>
       </c>
     </row>
     <row r="15">
@@ -934,25 +934,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1782949.13</v>
+        <v>1893604.81</v>
       </c>
       <c r="D15" t="n">
-        <v>1795029.64</v>
+        <v>1869391.58</v>
       </c>
       <c r="E15" t="n">
-        <v>75478.77</v>
+        <v>31543.56</v>
       </c>
       <c r="F15" t="n">
-        <v>38912.31</v>
+        <v>32025.3</v>
       </c>
       <c r="G15" t="n">
-        <v>1858427.9</v>
+        <v>1925148.37</v>
       </c>
       <c r="H15" t="n">
-        <v>1833941.95</v>
+        <v>1901416.88</v>
       </c>
       <c r="I15" t="n">
-        <v>24485.95</v>
+        <v>23731.49</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -970,25 +970,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1947894.45</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>44969.84</v>
       </c>
       <c r="E16" t="n">
-        <v>1020741.64</v>
+        <v>1084112.59</v>
       </c>
       <c r="F16" t="n">
-        <v>20269.33</v>
+        <v>32047.73</v>
       </c>
       <c r="G16" t="n">
-        <v>1020741.64</v>
+        <v>3032007.04</v>
       </c>
       <c r="H16" t="n">
-        <v>20269.33</v>
+        <v>77017.57000000001</v>
       </c>
       <c r="I16" t="n">
-        <v>1000472.31</v>
+        <v>2954989.47</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1006,28 +1006,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>410395.28</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>408797.81</v>
       </c>
       <c r="E17" t="n">
-        <v>166828.64</v>
+        <v>243967.47</v>
       </c>
       <c r="F17" t="n">
-        <v>124426.08</v>
+        <v>259972.74</v>
       </c>
       <c r="G17" t="n">
-        <v>166828.64</v>
+        <v>654362.75</v>
       </c>
       <c r="H17" t="n">
-        <v>124426.08</v>
+        <v>668770.55</v>
       </c>
       <c r="I17" t="n">
-        <v>42402.56</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>14407.8</v>
       </c>
     </row>
     <row r="18">
@@ -1042,25 +1042,25 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1215181.29</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>676294.02</v>
+        <v>446162.19</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>676294.02</v>
+        <v>1661343.48</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>676294.02</v>
+        <v>1661343.48</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1078,25 +1078,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1422839.37</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>133163.83</v>
       </c>
       <c r="E19" t="n">
-        <v>702241.87</v>
+        <v>604296.21</v>
       </c>
       <c r="F19" t="n">
-        <v>133163.83</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>702241.87</v>
+        <v>2027135.58</v>
       </c>
       <c r="H19" t="n">
         <v>133163.83</v>
       </c>
       <c r="I19" t="n">
-        <v>569078.04</v>
+        <v>1893971.75</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1114,25 +1114,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>20254</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>9386.190000000001</v>
+        <v>58903.74</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>9386.190000000001</v>
+        <v>79157.74000000001</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>9386.190000000001</v>
+        <v>79157.74000000001</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1150,25 +1150,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>218499.22</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>96761.45</v>
+        <v>119142.66</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>96761.45</v>
+        <v>337641.88</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>96761.45</v>
+        <v>337641.88</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1186,25 +1186,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>488024.45</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>10561</v>
       </c>
       <c r="E22" t="n">
-        <v>321748.82</v>
+        <v>140520.69</v>
       </c>
       <c r="F22" t="n">
-        <v>10561</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>321748.82</v>
+        <v>628545.14</v>
       </c>
       <c r="H22" t="n">
         <v>10561</v>
       </c>
       <c r="I22" t="n">
-        <v>311187.82</v>
+        <v>617984.14</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1222,25 +1222,25 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1555387.5</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>783437.09</v>
+        <v>731192.46</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>783437.09</v>
+        <v>2286579.96</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>783437.09</v>
+        <v>2286579.96</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1261,25 +1261,25 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>5352091.55</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>3303231.16</v>
+        <v>2803664.88</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>3303231.16</v>
+        <v>8155756.43</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>3303231.16</v>
+        <v>8155756.43</v>
       </c>
     </row>
     <row r="25">
@@ -1297,25 +1297,25 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>30607.01</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>14414.08</v>
+        <v>21746.37</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>14414.08</v>
+        <v>52353.38</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>14414.08</v>
+        <v>52353.38</v>
       </c>
     </row>
     <row r="26">
@@ -1333,25 +1333,25 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1529205.62</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>121590</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1650795.62</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1650795.62</v>
       </c>
     </row>
     <row r="27">
@@ -1369,25 +1369,25 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>156902.75</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>2607.94</v>
+        <v>48316.18</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>2607.94</v>
+        <v>205218.93</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>2607.94</v>
+        <v>205218.93</v>
       </c>
     </row>
     <row r="28">
@@ -1402,28 +1402,28 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>143724.83</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>6824707.91</v>
       </c>
       <c r="E28" t="n">
-        <v>143724.83</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>3632744.31</v>
+        <v>3136277.53</v>
       </c>
       <c r="G28" t="n">
         <v>143724.83</v>
       </c>
       <c r="H28" t="n">
-        <v>3632744.31</v>
+        <v>9960985.439999999</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>3489019.48</v>
+        <v>9817260.609999999</v>
       </c>
     </row>
     <row r="29">
@@ -1438,25 +1438,25 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>5720775.31</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>133163.83</v>
       </c>
       <c r="E29" t="n">
-        <v>3010648.52</v>
+        <v>2661954.34</v>
       </c>
       <c r="F29" t="n">
-        <v>133163.83</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>3010648.52</v>
+        <v>8382729.65</v>
       </c>
       <c r="H29" t="n">
         <v>133163.83</v>
       </c>
       <c r="I29" t="n">
-        <v>2877484.69</v>
+        <v>8249565.82</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1474,25 +1474,25 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>295034</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>142006.19</v>
+        <v>187585.93</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>142006.19</v>
+        <v>482619.93</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>142006.19</v>
+        <v>482619.93</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1510,25 +1510,25 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>320874.15</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>158340.78</v>
+        <v>146216.58</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>158340.78</v>
+        <v>467090.73</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>158340.78</v>
+        <v>467090.73</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -1546,25 +1546,25 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>488024.45</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>10561</v>
       </c>
       <c r="E32" t="n">
-        <v>321748.82</v>
+        <v>140520.68</v>
       </c>
       <c r="F32" t="n">
-        <v>10561</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>321748.82</v>
+        <v>628545.13</v>
       </c>
       <c r="H32" t="n">
         <v>10561</v>
       </c>
       <c r="I32" t="n">
-        <v>311187.82</v>
+        <v>617984.13</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1594,16 +1594,16 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>958498838.16</v>
+        <v>1015784383.09</v>
       </c>
       <c r="H33" t="n">
-        <v>960009634.36</v>
+        <v>1017295179.29</v>
       </c>
       <c r="I33" t="n">
-        <v>49121349.47</v>
+        <v>59969325.78</v>
       </c>
       <c r="J33" t="n">
-        <v>50632145.67</v>
+        <v>61480121.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>